<commit_message>
Har lavet SSD for UC6
Tidsregistrering opdateret
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Simon Nielsen.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Simon Nielsen.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -232,6 +232,63 @@
   </si>
   <si>
     <t>4.45t</t>
+  </si>
+  <si>
+    <t>Operationskontrakt 002</t>
+  </si>
+  <si>
+    <t>Rettet &amp; samlet Domain Model</t>
+  </si>
+  <si>
+    <t>3t</t>
+  </si>
+  <si>
+    <t>Fælles design OC3</t>
+  </si>
+  <si>
+    <t>Review OC2</t>
+  </si>
+  <si>
+    <t>2t</t>
+  </si>
+  <si>
+    <t>1t</t>
+  </si>
+  <si>
+    <t>Fraværende</t>
+  </si>
+  <si>
+    <t>1t 25m</t>
+  </si>
+  <si>
+    <t>Test Case OC6</t>
+  </si>
+  <si>
+    <t>SSD UC3</t>
+  </si>
+  <si>
+    <t>30m</t>
+  </si>
+  <si>
+    <t>Review af OC6 design</t>
+  </si>
+  <si>
+    <t>Review af SSD3</t>
+  </si>
+  <si>
+    <t>Implementeret test case for OC 6</t>
+  </si>
+  <si>
+    <t>Implementeret design for OC6</t>
+  </si>
+  <si>
+    <t>Lavet SSD for UC9</t>
+  </si>
+  <si>
+    <t>Krydscheck for UC6</t>
+  </si>
+  <si>
+    <t>SSD UC6</t>
   </si>
 </sst>
 </file>
@@ -285,10 +342,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,23 +673,25 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="48.85546875" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" customWidth="1"/>
     <col min="11" max="11" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -681,10 +740,10 @@
       <c r="F4" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>0.33680555555555558</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>0.54166666666666663</v>
       </c>
     </row>
@@ -693,10 +752,10 @@
       <c r="F5" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>0.58333333333333337</v>
       </c>
     </row>
@@ -717,10 +776,10 @@
       <c r="F7" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>0.34375</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>0.44791666666666669</v>
       </c>
     </row>
@@ -729,10 +788,10 @@
       <c r="F8" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>0.34375</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>0.44791666666666669</v>
       </c>
     </row>
@@ -741,10 +800,10 @@
       <c r="F9" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>0.34375</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>0.44791666666666669</v>
       </c>
       <c r="I9" t="s">
@@ -756,10 +815,10 @@
       <c r="F10" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>0.44791666666666669</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>0.47916666666666669</v>
       </c>
       <c r="I10" t="s">
@@ -771,10 +830,10 @@
       <c r="F11" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>0.52083333333333337</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>0.58333333333333337</v>
       </c>
       <c r="I11" t="s">
@@ -788,34 +847,246 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>42802</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="I13" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="I14" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+      <c r="I15" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>42804</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.34375</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42807</v>
+      </c>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42808</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>42809</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="I23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="I24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0.47222222222222227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.4770833333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.54513888888888895</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.57222222222222219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.59375</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.62847222222222221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0.64583333333333337</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Tidsregistrering opdateret Simon Nielsen
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Simon Nielsen.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Simon Nielsen.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -289,6 +289,21 @@
   </si>
   <si>
     <t>SSD UC6</t>
+  </si>
+  <si>
+    <t>Iterationsplan for iteration 4</t>
+  </si>
+  <si>
+    <t>SD og Klassediagram for erVaegtNormal</t>
+  </si>
+  <si>
+    <t>SD og Klassediagram for erArealNormal</t>
+  </si>
+  <si>
+    <t>review kode OC5</t>
+  </si>
+  <si>
+    <t>review kode OC7</t>
   </si>
 </sst>
 </file>
@@ -660,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,6 +1101,87 @@
       </c>
       <c r="H31" s="5">
         <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>42811</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.34375</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.35625000000000001</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0.39097222222222222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0.40625</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0.47569444444444442</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0.53125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Har lavet SD for OC13 beregnBoejningsmoment
tidsregistrering opdateret
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Simon Nielsen.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Simon Nielsen.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -304,6 +304,18 @@
   </si>
   <si>
     <t>review kode OC7</t>
+  </si>
+  <si>
+    <t>OC 14</t>
+  </si>
+  <si>
+    <t>SD &amp; DCD OC 9</t>
+  </si>
+  <si>
+    <t>SD &amp; DCD OC 8</t>
+  </si>
+  <si>
+    <t>SD &amp; DCD OC13</t>
   </si>
 </sst>
 </file>
@@ -675,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,6 +1194,53 @@
       </c>
       <c r="H38" s="5">
         <v>0.53125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>42814</v>
+      </c>
+      <c r="F41" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0.4375</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0.61597222222222225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0.64583333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Har lavet Test for Boejningsspaending og opdateret tidsregistrering
</commit_message>
<xml_diff>
--- a/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Simon Nielsen.xlsx
+++ b/Documentation/08 - Project Management/Tidsregistrering/Tidsregistrering i PTE projektet Simon Nielsen.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="104">
   <si>
     <t>Business-Process Analyst</t>
   </si>
@@ -331,6 +331,18 @@
   </si>
   <si>
     <t>Rettet Test Suite OC15</t>
+  </si>
+  <si>
+    <t>Implementeret OC12</t>
+  </si>
+  <si>
+    <t>Kode Review OC13</t>
+  </si>
+  <si>
+    <t>Hjalp med implementering af OC 15 &amp; 16</t>
+  </si>
+  <si>
+    <t>Test test og test</t>
   </si>
 </sst>
 </file>
@@ -702,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,7 +1309,7 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="49" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>26</v>
       </c>
@@ -1311,7 +1323,7 @@
         <v>0.60763888888888895</v>
       </c>
     </row>
-    <row r="50" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F50" t="s">
         <v>99</v>
       </c>
@@ -1320,6 +1332,64 @@
       </c>
       <c r="H50" s="5">
         <v>0.63194444444444442</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>42847</v>
+      </c>
+      <c r="F52" t="s">
+        <v>99</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="H52" s="5">
+        <v>0.36458333333333331</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>100</v>
+      </c>
+      <c r="G53" s="5">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="H53" s="5">
+        <v>0.38541666666666669</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>101</v>
+      </c>
+      <c r="G54" s="5">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="H54" s="5">
+        <v>0.4201388888888889</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>102</v>
+      </c>
+      <c r="G55" s="5">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="H55" s="5">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>103</v>
+      </c>
+      <c r="G56" s="5">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="H56" s="5">
+        <v>0.64583333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>